<commit_message>
Uploading temp sense, balancing, and more
</commit_message>
<xml_diff>
--- a/LTC6813/LTC6813 Summary.xlsx
+++ b/LTC6813/LTC6813 Summary.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\WFR\Custom BMS\Firmware\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\WFR\Custom BMS\Custom-BMS_25\LTC6813\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB92C891-97F3-4482-9C1A-76D8E2E7763F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39536585-3953-4D79-BBB3-96C29345D6DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1260" uniqueCount="872">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1261" uniqueCount="872">
   <si>
     <t>Register</t>
   </si>
@@ -2135,9 +2135,6 @@
   </si>
   <si>
     <t>PS[x]</t>
-  </si>
-  <si>
-    <t>Selects digital redundancy path</t>
   </si>
   <si>
     <t>Physical discharge timer enable</t>
@@ -2478,9 +2475,6 @@
     <t>Status register group diagnostic</t>
   </si>
   <si>
-    <t>ADCVSC</t>
-  </si>
-  <si>
     <t>CLRCELL</t>
   </si>
   <si>
@@ -2550,9 +2544,6 @@
     <t>0x054F</t>
   </si>
   <si>
-    <t>0x0567</t>
-  </si>
-  <si>
     <t>0x0711</t>
   </si>
   <si>
@@ -2665,6 +2656,38 @@
   </si>
   <si>
     <t>default all 1s!</t>
+  </si>
+  <si>
+    <t>ADCV</t>
+  </si>
+  <si>
+    <r>
+      <t>Selects digital redundancy path (</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>0x0360</t>
   </si>
 </sst>
 </file>
@@ -2782,13 +2805,13 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3071,8 +3094,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O125"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="K104" sqref="K104"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J7" sqref="J7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3092,24 +3115,24 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="12" t="s">
         <v>24</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="L1" s="11" t="s">
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="L1" s="12" t="s">
         <v>694</v>
       </c>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
@@ -3278,7 +3301,7 @@
         <v>695</v>
       </c>
       <c r="M5" s="1" t="s">
-        <v>704</v>
+        <v>703</v>
       </c>
       <c r="N5" s="1" t="s">
         <v>676</v>
@@ -3434,28 +3457,28 @@
       </c>
     </row>
     <row r="10" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A10" s="11" t="s">
+      <c r="A10" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
-      <c r="J10" s="11"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="12"/>
+      <c r="G10" s="12"/>
+      <c r="H10" s="12"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="12"/>
       <c r="L10" s="1" t="s">
         <v>692</v>
       </c>
       <c r="M10" s="1" t="s">
         <v>693</v>
       </c>
-      <c r="N10" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="O10" s="12"/>
+      <c r="N10" s="13" t="s">
+        <v>737</v>
+      </c>
+      <c r="O10" s="13"/>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
@@ -3580,12 +3603,12 @@
         <v>702</v>
       </c>
       <c r="M13" s="7" t="s">
-        <v>703</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="O13" s="12"/>
+        <v>870</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>737</v>
+      </c>
+      <c r="O13" s="13"/>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
@@ -3622,13 +3645,13 @@
         <v>74</v>
       </c>
       <c r="M14" s="7" t="s">
+        <v>704</v>
+      </c>
+      <c r="N14" s="7" t="s">
         <v>705</v>
       </c>
-      <c r="N14" s="7" t="s">
+      <c r="O14" s="7" t="s">
         <v>706</v>
-      </c>
-      <c r="O14" s="7" t="s">
-        <v>707</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -3663,10 +3686,10 @@
         <v>75</v>
       </c>
       <c r="L15" s="7" t="s">
+        <v>707</v>
+      </c>
+      <c r="M15" s="7" t="s">
         <v>708</v>
-      </c>
-      <c r="M15" s="7" t="s">
-        <v>709</v>
       </c>
       <c r="N15" s="6" t="s">
         <v>685</v>
@@ -3707,10 +3730,10 @@
         <v>75</v>
       </c>
       <c r="L16" s="7" t="s">
+        <v>709</v>
+      </c>
+      <c r="M16" s="7" t="s">
         <v>710</v>
-      </c>
-      <c r="M16" s="7" t="s">
-        <v>711</v>
       </c>
       <c r="N16" s="6" t="s">
         <v>685</v>
@@ -3751,10 +3774,10 @@
         <v>75</v>
       </c>
       <c r="L17" s="7" t="s">
+        <v>711</v>
+      </c>
+      <c r="M17" s="7" t="s">
         <v>712</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>713</v>
       </c>
       <c r="N17" s="6" t="s">
         <v>685</v>
@@ -3765,10 +3788,10 @@
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L18" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="M18" s="7" t="s">
         <v>714</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>715</v>
       </c>
       <c r="N18" s="6" t="s">
         <v>685</v>
@@ -3778,23 +3801,23 @@
       </c>
     </row>
     <row r="19" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A19" s="11" t="s">
+      <c r="A19" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="B19" s="11"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="11"/>
-      <c r="J19" s="11"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="12"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="12"/>
+      <c r="I19" s="12"/>
+      <c r="J19" s="12"/>
       <c r="L19" s="7" t="s">
+        <v>715</v>
+      </c>
+      <c r="M19" s="7" t="s">
         <v>716</v>
-      </c>
-      <c r="M19" s="7" t="s">
-        <v>717</v>
       </c>
       <c r="N19" s="6" t="s">
         <v>685</v>
@@ -3835,16 +3858,16 @@
         <v>9</v>
       </c>
       <c r="L20" s="7" t="s">
+        <v>717</v>
+      </c>
+      <c r="M20" s="7" t="s">
         <v>718</v>
       </c>
-      <c r="M20" s="7" t="s">
+      <c r="N20" s="7" t="s">
         <v>719</v>
       </c>
-      <c r="N20" s="7" t="s">
+      <c r="O20" s="7" t="s">
         <v>720</v>
-      </c>
-      <c r="O20" s="7" t="s">
-        <v>721</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -3879,16 +3902,16 @@
         <v>110</v>
       </c>
       <c r="L21" s="7" t="s">
+        <v>721</v>
+      </c>
+      <c r="M21" s="7" t="s">
         <v>722</v>
       </c>
-      <c r="M21" s="7" t="s">
+      <c r="N21" s="7" t="s">
         <v>723</v>
       </c>
-      <c r="N21" s="7" t="s">
+      <c r="O21" s="7" t="s">
         <v>724</v>
-      </c>
-      <c r="O21" s="7" t="s">
-        <v>725</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -3923,10 +3946,10 @@
         <v>122</v>
       </c>
       <c r="L22" s="7" t="s">
+        <v>725</v>
+      </c>
+      <c r="M22" s="7" t="s">
         <v>726</v>
-      </c>
-      <c r="M22" s="7" t="s">
-        <v>727</v>
       </c>
       <c r="N22" s="6" t="s">
         <v>685</v>
@@ -3970,7 +3993,7 @@
         <v>501</v>
       </c>
       <c r="M23" s="7" t="s">
-        <v>728</v>
+        <v>727</v>
       </c>
       <c r="N23" s="6" t="s">
         <v>685</v>
@@ -4014,13 +4037,13 @@
         <v>502</v>
       </c>
       <c r="M24" s="7" t="s">
-        <v>815</v>
+        <v>813</v>
       </c>
       <c r="N24" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="O24" s="7" t="s">
         <v>729</v>
-      </c>
-      <c r="O24" s="7" t="s">
-        <v>730</v>
       </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
@@ -4058,13 +4081,13 @@
         <v>503</v>
       </c>
       <c r="M25" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="N25" s="7" t="s">
         <v>731</v>
       </c>
-      <c r="N25" s="7" t="s">
+      <c r="O25" s="7" t="s">
         <v>732</v>
-      </c>
-      <c r="O25" s="7" t="s">
-        <v>733</v>
       </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
@@ -4096,44 +4119,44 @@
         <v>153</v>
       </c>
       <c r="J26" s="1" t="s">
-        <v>869</v>
+        <v>866</v>
       </c>
       <c r="L26" s="7" t="s">
+        <v>733</v>
+      </c>
+      <c r="M26" s="7" t="s">
         <v>734</v>
       </c>
-      <c r="M26" s="7" t="s">
-        <v>735</v>
-      </c>
-      <c r="N26" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="O26" s="12"/>
+      <c r="N26" s="13" t="s">
+        <v>737</v>
+      </c>
+      <c r="O26" s="13"/>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="L27" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="M27" s="7" t="s">
         <v>736</v>
       </c>
-      <c r="M27" s="7" t="s">
+      <c r="N27" s="13" t="s">
         <v>737</v>
       </c>
-      <c r="N27" s="12" t="s">
-        <v>738</v>
-      </c>
-      <c r="O27" s="12"/>
+      <c r="O27" s="13"/>
     </row>
     <row r="28" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A28" s="11" t="s">
+      <c r="A28" s="12" t="s">
         <v>154</v>
       </c>
-      <c r="B28" s="11"/>
-      <c r="C28" s="11"/>
-      <c r="D28" s="11"/>
-      <c r="E28" s="11"/>
-      <c r="F28" s="11"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="11"/>
+      <c r="B28" s="12"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="12"/>
+      <c r="H28" s="12"/>
+      <c r="I28" s="12"/>
+      <c r="J28" s="12"/>
       <c r="L28" s="4"/>
       <c r="M28" s="4"/>
       <c r="N28" s="4"/>
@@ -4398,18 +4421,18 @@
       <c r="O36" s="4"/>
     </row>
     <row r="37" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A37" s="11" t="s">
+      <c r="A37" s="12" t="s">
         <v>199</v>
       </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="11"/>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
-      <c r="F37" s="11"/>
-      <c r="G37" s="11"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="11"/>
-      <c r="J37" s="11"/>
+      <c r="B37" s="12"/>
+      <c r="C37" s="12"/>
+      <c r="D37" s="12"/>
+      <c r="E37" s="12"/>
+      <c r="F37" s="12"/>
+      <c r="G37" s="12"/>
+      <c r="H37" s="12"/>
+      <c r="I37" s="12"/>
+      <c r="J37" s="12"/>
       <c r="L37" s="4"/>
       <c r="M37" s="4"/>
       <c r="N37" s="4"/>
@@ -4674,18 +4697,18 @@
       <c r="O45" s="4"/>
     </row>
     <row r="46" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A46" s="11" t="s">
+      <c r="A46" s="12" t="s">
         <v>248</v>
       </c>
-      <c r="B46" s="11"/>
-      <c r="C46" s="11"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="11"/>
-      <c r="F46" s="11"/>
-      <c r="G46" s="11"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="11"/>
-      <c r="J46" s="11"/>
+      <c r="B46" s="12"/>
+      <c r="C46" s="12"/>
+      <c r="D46" s="12"/>
+      <c r="E46" s="12"/>
+      <c r="F46" s="12"/>
+      <c r="G46" s="12"/>
+      <c r="H46" s="12"/>
+      <c r="I46" s="12"/>
+      <c r="J46" s="12"/>
       <c r="L46" s="4"/>
       <c r="M46" s="4"/>
       <c r="N46" s="4"/>
@@ -4950,18 +4973,18 @@
       <c r="O54" s="4"/>
     </row>
     <row r="55" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A55" s="11" t="s">
+      <c r="A55" s="12" t="s">
         <v>297</v>
       </c>
-      <c r="B55" s="11"/>
-      <c r="C55" s="11"/>
-      <c r="D55" s="11"/>
-      <c r="E55" s="11"/>
-      <c r="F55" s="11"/>
-      <c r="G55" s="11"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="11"/>
-      <c r="J55" s="11"/>
+      <c r="B55" s="12"/>
+      <c r="C55" s="12"/>
+      <c r="D55" s="12"/>
+      <c r="E55" s="12"/>
+      <c r="F55" s="12"/>
+      <c r="G55" s="12"/>
+      <c r="H55" s="12"/>
+      <c r="I55" s="12"/>
+      <c r="J55" s="12"/>
       <c r="L55" s="4"/>
       <c r="M55" s="4"/>
       <c r="N55" s="4"/>
@@ -5226,18 +5249,18 @@
       <c r="O63" s="4"/>
     </row>
     <row r="64" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A64" s="11" t="s">
+      <c r="A64" s="12" t="s">
         <v>394</v>
       </c>
-      <c r="B64" s="11"/>
-      <c r="C64" s="11"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="11"/>
-      <c r="F64" s="11"/>
-      <c r="G64" s="11"/>
-      <c r="H64" s="11"/>
-      <c r="I64" s="11"/>
-      <c r="J64" s="11"/>
+      <c r="B64" s="12"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="12"/>
+      <c r="E64" s="12"/>
+      <c r="F64" s="12"/>
+      <c r="G64" s="12"/>
+      <c r="H64" s="12"/>
+      <c r="I64" s="12"/>
+      <c r="J64" s="12"/>
       <c r="L64" s="4"/>
       <c r="M64" s="4"/>
       <c r="N64" s="4"/>
@@ -5502,18 +5525,18 @@
       <c r="O72" s="4"/>
     </row>
     <row r="73" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A73" s="11" t="s">
+      <c r="A73" s="12" t="s">
         <v>395</v>
       </c>
-      <c r="B73" s="11"/>
-      <c r="C73" s="11"/>
-      <c r="D73" s="11"/>
-      <c r="E73" s="11"/>
-      <c r="F73" s="11"/>
-      <c r="G73" s="11"/>
-      <c r="H73" s="11"/>
-      <c r="I73" s="11"/>
-      <c r="J73" s="11"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="12"/>
+      <c r="D73" s="12"/>
+      <c r="E73" s="12"/>
+      <c r="F73" s="12"/>
+      <c r="G73" s="12"/>
+      <c r="H73" s="12"/>
+      <c r="I73" s="12"/>
+      <c r="J73" s="12"/>
       <c r="L73" s="4"/>
       <c r="M73" s="4"/>
       <c r="N73" s="4"/>
@@ -5778,18 +5801,18 @@
       <c r="O81" s="4"/>
     </row>
     <row r="82" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A82" s="11" t="s">
+      <c r="A82" s="12" t="s">
         <v>450</v>
       </c>
-      <c r="B82" s="11"/>
-      <c r="C82" s="11"/>
-      <c r="D82" s="11"/>
-      <c r="E82" s="11"/>
-      <c r="F82" s="11"/>
-      <c r="G82" s="11"/>
-      <c r="H82" s="11"/>
-      <c r="I82" s="11"/>
-      <c r="J82" s="11"/>
+      <c r="B82" s="12"/>
+      <c r="C82" s="12"/>
+      <c r="D82" s="12"/>
+      <c r="E82" s="12"/>
+      <c r="F82" s="12"/>
+      <c r="G82" s="12"/>
+      <c r="H82" s="12"/>
+      <c r="I82" s="12"/>
+      <c r="J82" s="12"/>
       <c r="L82" s="4"/>
       <c r="M82" s="4"/>
       <c r="N82" s="4"/>
@@ -6037,7 +6060,7 @@
         <v>501</v>
       </c>
       <c r="I89" s="1" t="s">
-        <v>814</v>
+        <v>812</v>
       </c>
       <c r="J89" s="1" t="s">
         <v>503</v>
@@ -6054,18 +6077,18 @@
       <c r="O90" s="4"/>
     </row>
     <row r="91" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A91" s="11" t="s">
+      <c r="A91" s="12" t="s">
         <v>504</v>
       </c>
-      <c r="B91" s="11"/>
-      <c r="C91" s="11"/>
-      <c r="D91" s="11"/>
-      <c r="E91" s="11"/>
-      <c r="F91" s="11"/>
-      <c r="G91" s="11"/>
-      <c r="H91" s="11"/>
-      <c r="I91" s="11"/>
-      <c r="J91" s="11"/>
+      <c r="B91" s="12"/>
+      <c r="C91" s="12"/>
+      <c r="D91" s="12"/>
+      <c r="E91" s="12"/>
+      <c r="F91" s="12"/>
+      <c r="G91" s="12"/>
+      <c r="H91" s="12"/>
+      <c r="I91" s="12"/>
+      <c r="J91" s="12"/>
       <c r="L91" s="4"/>
       <c r="M91" s="4"/>
       <c r="N91" s="4"/>
@@ -6330,18 +6353,18 @@
       <c r="O99" s="4"/>
     </row>
     <row r="100" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A100" s="11" t="s">
+      <c r="A100" s="12" t="s">
         <v>559</v>
       </c>
-      <c r="B100" s="11"/>
-      <c r="C100" s="11"/>
-      <c r="D100" s="11"/>
-      <c r="E100" s="11"/>
-      <c r="F100" s="11"/>
-      <c r="G100" s="11"/>
-      <c r="H100" s="11"/>
-      <c r="I100" s="11"/>
-      <c r="J100" s="11"/>
+      <c r="B100" s="12"/>
+      <c r="C100" s="12"/>
+      <c r="D100" s="12"/>
+      <c r="E100" s="12"/>
+      <c r="F100" s="12"/>
+      <c r="G100" s="12"/>
+      <c r="H100" s="12"/>
+      <c r="I100" s="12"/>
+      <c r="J100" s="12"/>
       <c r="L100" s="4"/>
       <c r="M100" s="4"/>
       <c r="N100" s="4"/>
@@ -6450,8 +6473,8 @@
       <c r="J103" s="1" t="s">
         <v>581</v>
       </c>
-      <c r="K103" s="13" t="s">
-        <v>871</v>
+      <c r="K103" s="11" t="s">
+        <v>868</v>
       </c>
       <c r="L103" s="4"/>
       <c r="M103" s="4"/>
@@ -6609,18 +6632,18 @@
       <c r="O108" s="4"/>
     </row>
     <row r="109" spans="1:15" ht="18" x14ac:dyDescent="0.35">
-      <c r="A109" s="11" t="s">
+      <c r="A109" s="12" t="s">
         <v>614</v>
       </c>
-      <c r="B109" s="11"/>
-      <c r="C109" s="11"/>
-      <c r="D109" s="11"/>
-      <c r="E109" s="11"/>
-      <c r="F109" s="11"/>
-      <c r="G109" s="11"/>
-      <c r="H109" s="11"/>
-      <c r="I109" s="11"/>
-      <c r="J109" s="11"/>
+      <c r="B109" s="12"/>
+      <c r="C109" s="12"/>
+      <c r="D109" s="12"/>
+      <c r="E109" s="12"/>
+      <c r="F109" s="12"/>
+      <c r="G109" s="12"/>
+      <c r="H109" s="12"/>
+      <c r="I109" s="12"/>
+      <c r="J109" s="12"/>
       <c r="L109" s="4"/>
       <c r="M109" s="4"/>
       <c r="N109" s="4"/>
@@ -6859,18 +6882,18 @@
       </c>
     </row>
     <row r="118" spans="1:10" ht="18" x14ac:dyDescent="0.35">
-      <c r="A118" s="11" t="s">
-        <v>841</v>
-      </c>
-      <c r="B118" s="11"/>
-      <c r="C118" s="11"/>
-      <c r="D118" s="11"/>
-      <c r="E118" s="11"/>
-      <c r="F118" s="11"/>
-      <c r="G118" s="11"/>
-      <c r="H118" s="11"/>
-      <c r="I118" s="11"/>
-      <c r="J118" s="11"/>
+      <c r="A118" s="12" t="s">
+        <v>838</v>
+      </c>
+      <c r="B118" s="12"/>
+      <c r="C118" s="12"/>
+      <c r="D118" s="12"/>
+      <c r="E118" s="12"/>
+      <c r="F118" s="12"/>
+      <c r="G118" s="12"/>
+      <c r="H118" s="12"/>
+      <c r="I118" s="12"/>
+      <c r="J118" s="12"/>
     </row>
     <row r="119" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A119" s="2" t="s">
@@ -6906,194 +6929,194 @@
     </row>
     <row r="120" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A120" s="1" t="s">
-        <v>842</v>
+        <v>839</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="G120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="H120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="I120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J120" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="121" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A121" s="1" t="s">
-        <v>843</v>
+        <v>840</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="G121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="H121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="I121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J121" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="122" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A122" s="1" t="s">
-        <v>844</v>
+        <v>841</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="G122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="H122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="I122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J122" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="123" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A123" s="1" t="s">
-        <v>845</v>
+        <v>842</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="D123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="E123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="F123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="G123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="H123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="I123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
       <c r="J123" s="6" t="s">
-        <v>848</v>
+        <v>845</v>
       </c>
     </row>
     <row r="124" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A124" s="1" t="s">
-        <v>846</v>
+        <v>843</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>856</v>
+        <v>853</v>
       </c>
       <c r="D124" s="1" t="s">
-        <v>855</v>
+        <v>852</v>
       </c>
       <c r="E124" s="1" t="s">
-        <v>854</v>
+        <v>851</v>
       </c>
       <c r="F124" s="1" t="s">
-        <v>853</v>
+        <v>850</v>
       </c>
       <c r="G124" s="1" t="s">
-        <v>852</v>
+        <v>849</v>
       </c>
       <c r="H124" s="1" t="s">
-        <v>851</v>
+        <v>848</v>
       </c>
       <c r="I124" s="1" t="s">
-        <v>850</v>
+        <v>847</v>
       </c>
       <c r="J124" s="1" t="s">
-        <v>849</v>
+        <v>846</v>
       </c>
     </row>
     <row r="125" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A125" s="1" t="s">
-        <v>847</v>
+        <v>844</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>102</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>864</v>
+        <v>861</v>
       </c>
       <c r="D125" s="1" t="s">
-        <v>863</v>
+        <v>860</v>
       </c>
       <c r="E125" s="1" t="s">
-        <v>862</v>
+        <v>859</v>
       </c>
       <c r="F125" s="1" t="s">
-        <v>861</v>
+        <v>858</v>
       </c>
       <c r="G125" s="1" t="s">
-        <v>860</v>
+        <v>857</v>
       </c>
       <c r="H125" s="1" t="s">
-        <v>859</v>
+        <v>856</v>
       </c>
       <c r="I125" s="1" t="s">
-        <v>858</v>
+        <v>855</v>
       </c>
       <c r="J125" s="1" t="s">
-        <v>857</v>
+        <v>854</v>
       </c>
     </row>
   </sheetData>
@@ -7120,6 +7143,7 @@
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -7127,8 +7151,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C9167C-FF39-4CDD-9CC0-7BECFC76D55A}">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="D24" sqref="D24"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7141,30 +7165,30 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>738</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>739</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>740</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>741</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>822</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>824</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>826</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>742</v>
       </c>
-      <c r="B2" s="1" t="s">
-        <v>743</v>
-      </c>
       <c r="C2" s="9" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>685</v>
@@ -7175,13 +7199,13 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>744</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>745</v>
-      </c>
       <c r="C3" s="9" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>685</v>
@@ -7192,13 +7216,13 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>746</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>747</v>
-      </c>
       <c r="C4" s="9" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>685</v>
@@ -7209,13 +7233,13 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>685</v>
@@ -7226,13 +7250,13 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>685</v>
@@ -7243,13 +7267,13 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>685</v>
@@ -7260,13 +7284,13 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C8" s="9" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>685</v>
@@ -7277,13 +7301,13 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>685</v>
@@ -7294,13 +7318,13 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>685</v>
@@ -7311,13 +7335,13 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>685</v>
@@ -7328,13 +7352,13 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>685</v>
@@ -7345,13 +7369,13 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="D13" s="6" t="s">
         <v>685</v>
@@ -7362,13 +7386,13 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>867</v>
+        <v>864</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>866</v>
+        <v>863</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>868</v>
+        <v>865</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>685</v>
@@ -7379,13 +7403,13 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>685</v>
@@ -7396,13 +7420,13 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>685</v>
@@ -7413,13 +7437,13 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="D17" s="6" t="s">
         <v>685</v>
@@ -7430,13 +7454,13 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="D18" s="6" t="s">
         <v>685</v>
@@ -7447,13 +7471,13 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="D19" s="6" t="s">
         <v>685</v>
@@ -7464,13 +7488,13 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="D20" s="6" t="s">
         <v>685</v>
@@ -7481,13 +7505,13 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>795</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>802</v>
+      </c>
+      <c r="C21" s="9" t="s">
         <v>796</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>803</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>797</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>685</v>
@@ -7498,13 +7522,13 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>797</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>798</v>
       </c>
-      <c r="B22" s="1" t="s">
+      <c r="C22" s="9" t="s">
         <v>799</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>800</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>685</v>
@@ -7515,47 +7539,47 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C23" s="9" t="s">
+        <v>821</v>
+      </c>
+      <c r="D23" s="9" t="s">
         <v>823</v>
       </c>
-      <c r="D23" s="9" t="s">
-        <v>825</v>
-      </c>
       <c r="E23" s="9" t="s">
-        <v>828</v>
+        <v>826</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="10" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C24" s="9" t="s">
+        <v>825</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>867</v>
+      </c>
+      <c r="E24" s="9" t="s">
         <v>827</v>
-      </c>
-      <c r="D24" s="9" t="s">
-        <v>870</v>
-      </c>
-      <c r="E24" s="9" t="s">
-        <v>829</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="10" t="s">
-        <v>821</v>
+        <v>819</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>822</v>
+        <v>820</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>830</v>
+        <v>828</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>685</v>
@@ -7566,13 +7590,13 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="10" t="s">
-        <v>839</v>
+        <v>836</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>865</v>
+        <v>862</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>840</v>
+        <v>837</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>685</v>
@@ -7583,45 +7607,47 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="10" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>831</v>
+        <v>829</v>
       </c>
       <c r="D27" s="9" t="s">
-        <v>832</v>
+        <v>830</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>829</v>
+        <v>827</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>809</v>
+        <v>869</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>833</v>
-      </c>
-      <c r="D28" s="9"/>
+        <v>871</v>
+      </c>
+      <c r="D28" s="6" t="s">
+        <v>685</v>
+      </c>
       <c r="E28" s="6" t="s">
         <v>685</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
-        <v>810</v>
+        <v>808</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>811</v>
+        <v>809</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>834</v>
+        <v>831</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>685</v>
@@ -7632,13 +7658,13 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
-        <v>812</v>
+        <v>810</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>813</v>
+        <v>811</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>835</v>
+        <v>832</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>685</v>
@@ -7649,13 +7675,13 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>816</v>
+        <v>814</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>817</v>
+        <v>815</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>836</v>
+        <v>833</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>685</v>
@@ -7669,10 +7695,10 @@
         <v>72</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>819</v>
+        <v>817</v>
       </c>
       <c r="C32" s="9" t="s">
-        <v>837</v>
+        <v>834</v>
       </c>
       <c r="D32" s="6" t="s">
         <v>685</v>
@@ -7683,13 +7709,13 @@
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1" t="s">
+        <v>816</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>818</v>
       </c>
-      <c r="B33" s="1" t="s">
-        <v>820</v>
-      </c>
       <c r="C33" s="9" t="s">
-        <v>838</v>
+        <v>835</v>
       </c>
       <c r="D33" s="6" t="s">
         <v>685</v>

</xml_diff>

<commit_message>
Pimped out error handling for LTC6813 read commands
</commit_message>
<xml_diff>
--- a/LTC6813/LTC6813 Summary.xlsx
+++ b/LTC6813/LTC6813 Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\WFR\Custom BMS\Custom-BMS_25\LTC6813\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2911D511-01D5-4F42-9E26-140B79AFC4D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C47A6E-BB1A-4F84-9DCB-1447323FDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="1" r:id="rId1"/>
@@ -2867,8 +2867,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView topLeftCell="A53" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+      <selection activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6653,6 +6653,11 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="A100:J100"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="A73:J73"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A64:J64"/>
@@ -6666,11 +6671,6 @@
     <mergeCell ref="A55:J55"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A10:J10"/>
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="A100:J100"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="A73:J73"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6681,8 +6681,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C9167C-FF39-4CDD-9CC0-7BECFC76D55A}">
   <dimension ref="A1:E28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
PCB temp sense & CAN message list
</commit_message>
<xml_diff>
--- a/LTC6813/LTC6813 Summary.xlsx
+++ b/LTC6813/LTC6813 Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\WFR\Custom BMS\Custom-BMS_25\LTC6813\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C47A6E-BB1A-4F84-9DCB-1447323FDA70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A57B72D1-30CA-4962-8198-C72DE68FCC0C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1164" uniqueCount="807">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="813">
   <si>
     <t>Register</t>
   </si>
@@ -2470,6 +2470,24 @@
   </si>
   <si>
     <t>Reads auxiliary register group D</t>
+  </si>
+  <si>
+    <t>Aux register diagnostic</t>
+  </si>
+  <si>
+    <t>AXST</t>
+  </si>
+  <si>
+    <t>ADOL</t>
+  </si>
+  <si>
+    <t>Overlap cell measurement diagnostic</t>
+  </si>
+  <si>
+    <t>AXOW</t>
+  </si>
+  <si>
+    <t>Open circuit test on GPIO</t>
   </si>
 </sst>
 </file>
@@ -2867,7 +2885,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A96" workbookViewId="0">
+    <sheetView topLeftCell="A46" workbookViewId="0">
       <selection activeCell="M107" sqref="M107"/>
     </sheetView>
   </sheetViews>
@@ -6653,11 +6671,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="A100:J100"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="A73:J73"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A64:J64"/>
@@ -6671,6 +6684,11 @@
     <mergeCell ref="A55:J55"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="A100:J100"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="A73:J73"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6679,10 +6697,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C9167C-FF39-4CDD-9CC0-7BECFC76D55A}">
-  <dimension ref="A1:E28"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6984,64 +7002,58 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="10" t="s">
-        <v>570</v>
+        <v>811</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>572</v>
-      </c>
-      <c r="C18" s="9" t="s">
-        <v>589</v>
-      </c>
-      <c r="D18" s="9" t="s">
-        <v>591</v>
-      </c>
-      <c r="E18" s="9" t="s">
-        <v>594</v>
-      </c>
+        <v>812</v>
+      </c>
+      <c r="C18" s="9"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="10" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>804</v>
+        <v>591</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>595</v>
+        <v>594</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="10" t="s">
+        <v>573</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>575</v>
+      </c>
+      <c r="C20" s="9" t="s">
+        <v>593</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>804</v>
+      </c>
+      <c r="E20" s="9" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="10" t="s">
         <v>802</v>
       </c>
-      <c r="B20" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>588</v>
       </c>
-      <c r="C20" s="9" t="s">
+      <c r="C21" s="9" t="s">
         <v>803</v>
-      </c>
-      <c r="D20" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="E20" s="6" t="s">
-        <v>477</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A21" s="1" t="s">
-        <v>801</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>805</v>
-      </c>
-      <c r="C21" s="9" t="s">
-        <v>800</v>
       </c>
       <c r="D21" s="6" t="s">
         <v>477</v>
@@ -7052,30 +7064,24 @@
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="10" t="s">
-        <v>574</v>
+        <v>809</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>576</v>
-      </c>
-      <c r="C22" s="9" t="s">
-        <v>596</v>
-      </c>
-      <c r="D22" s="9" t="s">
-        <v>597</v>
-      </c>
-      <c r="E22" s="9" t="s">
-        <v>595</v>
-      </c>
+        <v>810</v>
+      </c>
+      <c r="C22" s="9"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A23" s="1" t="s">
-        <v>798</v>
+      <c r="A23" s="10" t="s">
+        <v>808</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>571</v>
+        <v>807</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>799</v>
+        <v>800</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>477</v>
@@ -7085,31 +7091,31 @@
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A24" s="1" t="s">
-        <v>577</v>
+      <c r="A24" s="10" t="s">
+        <v>574</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
       <c r="C24" s="9" t="s">
-        <v>598</v>
-      </c>
-      <c r="D24" s="6" t="s">
-        <v>477</v>
-      </c>
-      <c r="E24" s="6" t="s">
-        <v>477</v>
+        <v>596</v>
+      </c>
+      <c r="D24" s="9" t="s">
+        <v>597</v>
+      </c>
+      <c r="E24" s="9" t="s">
+        <v>595</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1" t="s">
-        <v>579</v>
+        <v>801</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>580</v>
+        <v>805</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>599</v>
+        <v>800</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>477</v>
@@ -7119,14 +7125,14 @@
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A26" s="10" t="s">
-        <v>583</v>
+      <c r="A26" s="1" t="s">
+        <v>798</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>584</v>
+        <v>571</v>
       </c>
       <c r="C26" s="9" t="s">
-        <v>600</v>
+        <v>799</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>477</v>
@@ -7137,13 +7143,13 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1" t="s">
-        <v>72</v>
+        <v>577</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>586</v>
+        <v>578</v>
       </c>
       <c r="C27" s="9" t="s">
-        <v>601</v>
+        <v>598</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>477</v>
@@ -7154,18 +7160,69 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>585</v>
+        <v>579</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>587</v>
+        <v>580</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>602</v>
+        <v>599</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>477</v>
       </c>
       <c r="E28" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="10" t="s">
+        <v>583</v>
+      </c>
+      <c r="B29" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>600</v>
+      </c>
+      <c r="D29" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E29" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B30" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>601</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B31" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C31" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="D31" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E31" s="6" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>

<commit_message>
manual balancing + much of automatic (not tested!)
</commit_message>
<xml_diff>
--- a/LTC6813/LTC6813 Summary.xlsx
+++ b/LTC6813/LTC6813 Summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\My Documents\WFR\Custom BMS\Custom-BMS_25\LTC6813\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96226D6C-5B3A-4CBC-BC2C-19D9E8608A44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC79CD4-1E2A-4FCF-A917-896112B3CB74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-23148" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Registers" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1173" uniqueCount="813">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1178" uniqueCount="816">
   <si>
     <t>Register</t>
   </si>
@@ -2488,6 +2488,15 @@
   </si>
   <si>
     <t>Open circuit test on GPIO</t>
+  </si>
+  <si>
+    <t>CLRAUX</t>
+  </si>
+  <si>
+    <t>0x0712</t>
+  </si>
+  <si>
+    <t>Clears aux register groups</t>
   </si>
 </sst>
 </file>
@@ -2885,8 +2894,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:O116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="L95" sqref="L95"/>
+    <sheetView topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F92" sqref="F92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6671,11 +6680,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="A91:J91"/>
-    <mergeCell ref="A100:J100"/>
-    <mergeCell ref="A109:J109"/>
-    <mergeCell ref="A82:J82"/>
-    <mergeCell ref="A73:J73"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="A19:J19"/>
     <mergeCell ref="A64:J64"/>
@@ -6689,6 +6693,11 @@
     <mergeCell ref="A55:J55"/>
     <mergeCell ref="A1:J1"/>
     <mergeCell ref="A10:J10"/>
+    <mergeCell ref="A91:J91"/>
+    <mergeCell ref="A100:J100"/>
+    <mergeCell ref="A109:J109"/>
+    <mergeCell ref="A82:J82"/>
+    <mergeCell ref="A73:J73"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6697,10 +6706,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0C9167C-FF39-4CDD-9CC0-7BECFC76D55A}">
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7160,13 +7169,13 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
-        <v>579</v>
+        <v>813</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>580</v>
+        <v>815</v>
       </c>
       <c r="C28" s="9" t="s">
-        <v>599</v>
+        <v>814</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>477</v>
@@ -7176,14 +7185,14 @@
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A29" s="10" t="s">
-        <v>583</v>
+      <c r="A29" s="1" t="s">
+        <v>579</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>600</v>
+        <v>599</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>477</v>
@@ -7193,14 +7202,14 @@
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>72</v>
+      <c r="A30" s="10" t="s">
+        <v>583</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
       <c r="C30" s="9" t="s">
-        <v>601</v>
+        <v>600</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>477</v>
@@ -7211,18 +7220,35 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
-        <v>585</v>
+        <v>72</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>587</v>
+        <v>586</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>602</v>
+        <v>601</v>
       </c>
       <c r="D31" s="6" t="s">
         <v>477</v>
       </c>
       <c r="E31" s="6" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="B32" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="C32" s="9" t="s">
+        <v>602</v>
+      </c>
+      <c r="D32" s="6" t="s">
+        <v>477</v>
+      </c>
+      <c r="E32" s="6" t="s">
         <v>477</v>
       </c>
     </row>

</xml_diff>